<commit_message>
added images for accuracy in readme
</commit_message>
<xml_diff>
--- a/S6/BackPropagationExcel.xlsx
+++ b/S6/BackPropagationExcel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Deep Learning\Assignments\session 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Deep Learning\Assignments\ERAV1\S6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621D8C3D-EAF9-416D-91EC-6FDB73807984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBF02A0-7BC6-4054-9678-B9255C9DE5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +285,13 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -295,8 +302,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -310,22 +316,23 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -335,7 +342,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -343,8 +349,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4333,8 +4341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:AF86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J86" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4365,13 +4373,13 @@
       </c>
     </row>
     <row r="6" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0.05</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="5"/>
       <c r="K6" t="s">
         <v>7</v>
       </c>
@@ -4412,7 +4420,7 @@
       </c>
     </row>
     <row r="13" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>0.1</v>
       </c>
       <c r="K13" t="s">
@@ -4431,10 +4439,10 @@
       </c>
     </row>
     <row r="15" spans="4:19" x14ac:dyDescent="0.25">
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="5"/>
       <c r="P15" t="s">
         <v>21</v>
       </c>
@@ -4463,12 +4471,12 @@
       </c>
     </row>
     <row r="20" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="P20" s="5" t="s">
+      <c r="P20" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="P21" s="5" t="s">
+      <c r="P21" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4476,7 +4484,7 @@
       <c r="C22" t="s">
         <v>32</v>
       </c>
-      <c r="P22" s="5" t="s">
+      <c r="P22" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -4503,7 +4511,7 @@
       <c r="I25" t="s">
         <v>33</v>
       </c>
-      <c r="R25" s="5" t="s">
+      <c r="R25" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4511,7 +4519,7 @@
       <c r="C26" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>36</v>
       </c>
       <c r="R26" t="s">
@@ -4525,7 +4533,7 @@
       <c r="I27" t="s">
         <v>39</v>
       </c>
-      <c r="R27" s="5" t="s">
+      <c r="R27" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4546,7 +4554,7 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
-      <c r="I30" s="5"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
@@ -4560,7 +4568,7 @@
       <c r="C32" t="s">
         <v>53</v>
       </c>
-      <c r="P32" s="5" t="s">
+      <c r="P32" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4573,7 +4581,7 @@
       <c r="C34" t="s">
         <v>54</v>
       </c>
-      <c r="P34" s="5" t="s">
+      <c r="P34" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4585,101 +4593,101 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="J40" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K40" s="3" t="s">
+      <c r="K40" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M40" s="3" t="s">
+      <c r="M40" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N40" s="3" t="s">
+      <c r="N40" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O40" s="3" t="s">
+      <c r="O40" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="P40" s="3" t="s">
+      <c r="P40" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q40" s="3" t="s">
+      <c r="Q40" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="R40" s="3" t="s">
+      <c r="R40" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="S40" s="3" t="s">
+      <c r="S40" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="T40" s="3" t="s">
+      <c r="T40" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U40" s="3" t="s">
+      <c r="U40" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="V40" s="3" t="s">
+      <c r="V40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="W40" s="3" t="s">
+      <c r="W40" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="X40" s="3" t="s">
+      <c r="X40" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Y40" s="3" t="s">
+      <c r="Y40" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Z40" s="3" t="s">
+      <c r="Z40" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="AA40" s="3" t="s">
+      <c r="AA40" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="AB40" s="3" t="s">
+      <c r="AB40" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AC40" s="3" t="s">
+      <c r="AC40" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="AD40" s="3" t="s">
+      <c r="AD40" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AE40" s="3" t="s">
+      <c r="AE40" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AF40" s="3" t="s">
+      <c r="AF40" s="6" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>